<commit_message>
Version 0.7; device.device_count added
</commit_message>
<xml_diff>
--- a/pf2050_data_standard_sample.xlsx
+++ b/pf2050_data_standard_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\data-standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06E1025-13B8-4556-A486-5AE593B20E49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4274D3A-E0E3-4ED8-AEAE-D86BC02536B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{64A28DED-81D2-4CDB-A055-0A4AAA730851}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{64A28DED-81D2-4CDB-A055-0A4AAA730851}"/>
   </bookViews>
   <sheets>
     <sheet name="Examples" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="78">
   <si>
     <t>Example Data Set 1</t>
   </si>
@@ -1027,6 +1027,32 @@
         <scheme val="minor"/>
       </rPr>
       <t>.person_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>device</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_count</t>
     </r>
   </si>
 </sst>
@@ -1409,13 +1435,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F4A553-C01A-4682-842C-40C1FC09DA16}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,194 +1953,215 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1</v>
+      </c>
+      <c r="G22" s="6">
+        <v>20</v>
+      </c>
+      <c r="H22" s="6">
+        <v>20</v>
+      </c>
+      <c r="I22" s="6">
+        <v>20</v>
+      </c>
+      <c r="J22" s="6">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="6">
-        <v>456</v>
-      </c>
-      <c r="D23" s="6">
-        <v>456</v>
-      </c>
-      <c r="E23" s="6">
-        <v>456</v>
-      </c>
-      <c r="F23" s="6">
-        <v>456</v>
+      <c r="C23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="H23" s="6"/>
-      <c r="I23" s="6">
-        <v>456</v>
-      </c>
-      <c r="J23" s="6">
-        <v>456</v>
+      <c r="I23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="C24" s="6">
+        <v>456</v>
+      </c>
+      <c r="D24" s="6">
+        <v>456</v>
+      </c>
+      <c r="E24" s="6">
+        <v>456</v>
+      </c>
+      <c r="F24" s="6">
+        <v>456</v>
       </c>
       <c r="H24" s="6"/>
-      <c r="I24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>12</v>
+      <c r="I24" s="6">
+        <v>456</v>
+      </c>
+      <c r="J24" s="6">
+        <v>456</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="6">
-        <v>28</v>
-      </c>
-      <c r="F26" s="6">
-        <v>28</v>
-      </c>
-      <c r="I26">
-        <v>2800</v>
-      </c>
-      <c r="J26">
-        <v>1400</v>
+        <v>19</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="6">
-        <v>789</v>
-      </c>
-      <c r="G27" s="6">
-        <v>789</v>
-      </c>
-      <c r="H27">
-        <v>123</v>
+      <c r="C27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="6">
+        <v>28</v>
+      </c>
+      <c r="F27" s="6">
+        <v>28</v>
+      </c>
+      <c r="I27">
+        <v>2800</v>
+      </c>
+      <c r="J27">
+        <v>1400</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>61</v>
+        <v>28</v>
+      </c>
+      <c r="C28" s="6">
+        <v>789</v>
+      </c>
+      <c r="G28" s="6">
+        <v>789</v>
+      </c>
+      <c r="H28">
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="C29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>27</v>
@@ -2125,55 +2172,66 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="6">
-        <v>1</v>
-      </c>
-      <c r="G32" s="6">
-        <v>56</v>
-      </c>
-      <c r="H32">
-        <v>17</v>
+      <c r="C32" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="6" t="b">
+      <c r="C33" s="6">
         <v>1</v>
       </c>
-      <c r="G33" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="6" t="b">
-        <v>1</v>
+      <c r="G33" s="6">
+        <v>56</v>
+      </c>
+      <c r="H33">
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2386,18 +2444,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2419,18 +2477,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D965EBF-0A09-409E-9A60-064A182B9D88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A951D2D-01AB-404A-B47B-312EC1665A5E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D965EBF-0A09-409E-9A60-064A182B9D88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version 0.8; UUID overhaul
</commit_message>
<xml_diff>
--- a/pf2050_data_standard_sample.xlsx
+++ b/pf2050_data_standard_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\data-standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4274D3A-E0E3-4ED8-AEAE-D86BC02536B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879078BC-9272-4A1C-A308-2F26E938C3D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{64A28DED-81D2-4CDB-A055-0A4AAA730851}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{64A28DED-81D2-4CDB-A055-0A4AAA730851}"/>
   </bookViews>
   <sheets>
     <sheet name="Examples" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="83">
   <si>
     <t>Example Data Set 1</t>
   </si>
@@ -260,58 +260,6 @@
   </si>
   <si>
     <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>device</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.device_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>device</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.device_model</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>pf2050_data_standard.report.device.</t>
     </r>
     <r>
@@ -360,318 +308,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>.status_value</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.device.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.device.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_id</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.device.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.device.substance.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance_status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.status_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.device.substance.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance_status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.status_value</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_id</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.common_name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.scientific_name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.age</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.sex</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.count</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.target</t>
     </r>
   </si>
   <si>
@@ -948,7 +584,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.location</t>
+      <t>.person_uuid</t>
     </r>
   </si>
   <si>
@@ -964,6 +600,162 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>person</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.person_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>person</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.person_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>device</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_count</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>device</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>device</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>device</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_model</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>report</t>
     </r>
     <r>
@@ -974,7 +766,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.person_uuid</t>
+      <t>.location_uuid</t>
     </r>
   </si>
   <si>
@@ -990,17 +782,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>person</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.person_uuid</t>
+      <t>location</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.location_uuid</t>
     </r>
   </si>
   <si>
@@ -1016,17 +808,95 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>person</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.person_name</t>
+      <t>location</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.location_wkt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_name</t>
     </r>
   </si>
   <si>
@@ -1042,17 +912,277 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>device</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.device_count</t>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.substance.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance_status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.status_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.substance.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance_status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.status_value</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_age</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_sex</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_count</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_target</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_common_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_scientific_name</t>
     </r>
   </si>
 </sst>
@@ -1435,13 +1565,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F4A553-C01A-4682-842C-40C1FC09DA16}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,7 +1585,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>30</v>
@@ -1473,16 +1603,16 @@
         <v>24</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1519,7 +1649,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>27</v>
@@ -1557,33 +1687,33 @@
         <v>26</v>
       </c>
       <c r="C4" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D4" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E4" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="F4" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G4" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="H4" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="I4" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="J4" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>27</v>
@@ -1591,7 +1721,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>27</v>
@@ -1599,7 +1729,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>27</v>
@@ -1607,7 +1737,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>27</v>
@@ -1615,7 +1745,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>27</v>
@@ -1623,7 +1753,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>27</v>
@@ -1646,7 +1776,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>27</v>
@@ -1669,170 +1799,170 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>7</v>
@@ -1846,12 +1976,7 @@
       <c r="F17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="H17" s="6"/>
       <c r="I17" s="6" t="s">
         <v>7</v>
       </c>
@@ -1861,377 +1986,501 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="H18" s="6"/>
       <c r="I18" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>8</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H19" s="6"/>
       <c r="I19" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6">
-        <v>1</v>
-      </c>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6">
-        <v>1</v>
-      </c>
-      <c r="G22" s="6">
-        <v>20</v>
-      </c>
-      <c r="H22" s="6">
-        <v>20</v>
-      </c>
-      <c r="I22" s="6">
-        <v>20</v>
-      </c>
-      <c r="J22" s="6">
-        <v>20</v>
-      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="I23" s="6" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="6">
-        <v>456</v>
-      </c>
-      <c r="D24" s="6">
-        <v>456</v>
-      </c>
-      <c r="E24" s="6">
-        <v>456</v>
-      </c>
-      <c r="F24" s="6">
-        <v>456</v>
-      </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6">
-        <v>456</v>
-      </c>
-      <c r="J24" s="6">
-        <v>456</v>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="I25" s="6" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="I26" s="6" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="6">
-        <v>28</v>
-      </c>
-      <c r="F27" s="6">
-        <v>28</v>
-      </c>
-      <c r="I27">
-        <v>2800</v>
-      </c>
-      <c r="J27">
-        <v>1400</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="6">
-        <v>789</v>
-      </c>
-      <c r="G28" s="6">
-        <v>789</v>
-      </c>
-      <c r="H28">
-        <v>123</v>
+        <v>27</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>61</v>
+        <v>9</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>15</v>
+      <c r="C31" s="6">
+        <v>1</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
+      <c r="F31" s="6">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6">
+        <v>20</v>
+      </c>
+      <c r="H31" s="6">
+        <v>20</v>
+      </c>
+      <c r="I31" s="6">
+        <v>20</v>
+      </c>
+      <c r="J31" s="6">
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="6">
+        <v>28</v>
+      </c>
+      <c r="F34" s="6">
+        <v>28</v>
+      </c>
+      <c r="I34">
+        <v>2800</v>
+      </c>
+      <c r="J34">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" s="4" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C37" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G38" s="6">
         <v>56</v>
       </c>
-      <c r="H33">
+      <c r="H38">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="4" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="6" t="b">
+      <c r="C39" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="G34" s="6" t="b">
+      <c r="G39" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="H34" s="6" t="b">
+      <c r="H39" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="4" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2265,7 +2514,7 @@
     </row>
     <row r="2" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2274,6 +2523,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001841EF6FFA7F374192AC0CC924A6F925" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2f87bbec06d9a4ef9af4a600d8d8ff8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3eb05d59-0ff5-49fb-8192-aa16a29e7496" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f152831af84cbb245f73b2e8081d3a2" ns3:_="">
     <xsd:import namespace="3eb05d59-0ff5-49fb-8192-aa16a29e7496"/>
@@ -2443,22 +2707,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D965EBF-0A09-409E-9A60-064A182B9D88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A951D2D-01AB-404A-B47B-312EC1665A5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5603EAEC-0B1D-41E0-A2B7-A3AB9F295DD2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2474,21 +2740,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A951D2D-01AB-404A-B47B-312EC1665A5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D965EBF-0A09-409E-9A60-064A182B9D88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version 0.9; device model changes
</commit_message>
<xml_diff>
--- a/pf2050_data_standard_sample.xlsx
+++ b/pf2050_data_standard_sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\data-standard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\data-standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879078BC-9272-4A1C-A308-2F26E938C3D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC114D1-CA68-49C4-BAA8-FE815A41EC51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{64A28DED-81D2-4CDB-A055-0A4AAA730851}"/>
+    <workbookView xWindow="28680" yWindow="285" windowWidth="25440" windowHeight="15540" xr2:uid="{64A28DED-81D2-4CDB-A055-0A4AAA730851}"/>
   </bookViews>
   <sheets>
     <sheet name="Examples" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="85">
   <si>
     <t>Example Data Set 1</t>
   </si>
@@ -714,7 +714,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.device_type</t>
+      <t>.device_model</t>
     </r>
   </si>
   <si>
@@ -730,17 +730,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>device</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.device_model</t>
+      <t>report</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.location_uuid</t>
     </r>
   </si>
   <si>
@@ -756,7 +756,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>report</t>
+      <t>location</t>
     </r>
     <r>
       <rPr>
@@ -792,7 +792,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.location_uuid</t>
+      <t>.location_wkt</t>
     </r>
   </si>
   <si>
@@ -808,17 +808,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>location</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.location_wkt</t>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_uuid</t>
     </r>
   </si>
   <si>
@@ -844,11 +844,115 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>.substance_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>.substance_uuid</t>
     </r>
   </si>
   <si>
     <r>
+      <t>pf2050_data_standard.report.substance.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance_status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.status_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.substance.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance_status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.status_value</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>pf2050_data_standard.</t>
     </r>
     <r>
@@ -860,17 +964,147 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_type</t>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_age</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_sex</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_count</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_target</t>
     </r>
   </si>
   <si>
@@ -886,95 +1120,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.substance.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance_status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.status_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.substance.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance_status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.status_value</t>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_common_name</t>
     </r>
   </si>
   <si>
@@ -1000,137 +1156,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.species_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_age</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_sex</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_count</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_target</t>
+      <t>.species_scientific_name</t>
     </r>
   </si>
   <si>
@@ -1146,17 +1172,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_common_name</t>
+      <t>device_model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_model_uuid</t>
     </r>
   </si>
   <si>
@@ -1172,17 +1198,43 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_scientific_name</t>
+      <t>device_model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_model_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>device_model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_model_name</t>
     </r>
   </si>
 </sst>
@@ -1565,13 +1617,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F4A553-C01A-4682-842C-40C1FC09DA16}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,28 +1739,28 @@
         <v>26</v>
       </c>
       <c r="C4" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D4" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E4" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="F4" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G4" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="H4" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="I4" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="J4" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1799,10 +1851,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
@@ -1831,7 +1883,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
@@ -1863,10 +1915,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>7</v>
@@ -1895,71 +1947,71 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>28</v>
@@ -1976,7 +2028,12 @@
       <c r="F17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="I17" s="6" t="s">
         <v>7</v>
       </c>
@@ -1986,501 +2043,560 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="I18" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>47</v>
+        <v>12</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="6">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6">
-        <v>1</v>
-      </c>
-      <c r="E31" s="6">
-        <v>1</v>
-      </c>
-      <c r="F31" s="6">
-        <v>1</v>
-      </c>
-      <c r="G31" s="6">
-        <v>20</v>
-      </c>
-      <c r="H31" s="6">
-        <v>20</v>
-      </c>
-      <c r="I31" s="6">
-        <v>20</v>
-      </c>
-      <c r="J31" s="6">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6">
+        <v>1</v>
+      </c>
+      <c r="F33" s="6">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6">
+        <v>20</v>
+      </c>
+      <c r="H33" s="6">
+        <v>20</v>
+      </c>
+      <c r="I33" s="6">
+        <v>20</v>
+      </c>
+      <c r="J33" s="6">
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="6">
-        <v>28</v>
-      </c>
-      <c r="F34" s="6">
-        <v>28</v>
-      </c>
-      <c r="I34">
-        <v>2800</v>
-      </c>
-      <c r="J34">
-        <v>1400</v>
+        <v>7</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="6">
+        <v>28</v>
+      </c>
+      <c r="F36" s="6">
+        <v>28</v>
+      </c>
+      <c r="I36">
+        <v>2800</v>
+      </c>
+      <c r="J36">
+        <v>1400</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="6">
-        <v>1</v>
-      </c>
-      <c r="G38" s="6">
-        <v>56</v>
-      </c>
-      <c r="H38">
-        <v>17</v>
+      <c r="C38" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="6" t="b">
-        <v>1</v>
+      <c r="C39" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="6">
+        <v>1</v>
+      </c>
+      <c r="G40" s="6">
+        <v>56</v>
+      </c>
+      <c r="H40">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2523,21 +2639,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001841EF6FFA7F374192AC0CC924A6F925" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2f87bbec06d9a4ef9af4a600d8d8ff8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3eb05d59-0ff5-49fb-8192-aa16a29e7496" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f152831af84cbb245f73b2e8081d3a2" ns3:_="">
     <xsd:import namespace="3eb05d59-0ff5-49fb-8192-aa16a29e7496"/>
@@ -2707,24 +2808,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D965EBF-0A09-409E-9A60-064A182B9D88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A951D2D-01AB-404A-B47B-312EC1665A5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5603EAEC-0B1D-41E0-A2B7-A3AB9F295DD2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2740,4 +2839,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A951D2D-01AB-404A-B47B-312EC1665A5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D965EBF-0A09-409E-9A60-064A182B9D88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version 0.10; updated after discussion 4/3/21
</commit_message>
<xml_diff>
--- a/pf2050_data_standard_sample.xlsx
+++ b/pf2050_data_standard_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\data-standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC114D1-CA68-49C4-BAA8-FE815A41EC51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B65A87-24F1-4669-A553-626926B089CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="285" windowWidth="25440" windowHeight="15540" xr2:uid="{64A28DED-81D2-4CDB-A055-0A4AAA730851}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{64A28DED-81D2-4CDB-A055-0A4AAA730851}"/>
   </bookViews>
   <sheets>
     <sheet name="Examples" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="91">
   <si>
     <t>Example Data Set 1</t>
   </si>
@@ -730,6 +730,529 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>location</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.location_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>location</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.location_wkt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.substance_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.substance.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance_status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.status_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.substance.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>substance_status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.status_value</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_age</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_sex</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_count</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.report.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_target</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_common_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.species_scientific_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>device_model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_model_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>device_model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_model_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>device_model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.device_model_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>location</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.location_attribute</t>
+    </r>
+  </si>
+  <si>
+    <t>On Tree</t>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>report</t>
     </r>
     <r>
@@ -740,501 +1263,88 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.location_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>location</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.location_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>location</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.location_wkt</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.substance_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.substance.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance_status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.status_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.substance.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>substance_status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.status_value</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_age</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_sex</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_count</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.report.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_target</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_common_name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>species</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.species_scientific_name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>device_model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.device_model_uuid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>device_model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.device_model_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pf2050_data_standard.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>device_model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.device_model_name</t>
+      <t>.location.location_uuid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>report</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.location.location_wkt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>report</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.location.location_attribute</t>
+    </r>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <r>
+      <t>pf2050_data_standard.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>report</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.data_standard_version</t>
     </r>
   </si>
 </sst>
@@ -1285,7 +1395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1301,6 +1411,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1617,13 +1730,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F4A553-C01A-4682-842C-40C1FC09DA16}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,29 +1851,29 @@
       <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0.9</v>
+      <c r="C4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1851,10 +1964,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
@@ -1883,7 +1996,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
@@ -1915,66 +2028,57 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1982,71 +2086,71 @@
         <v>83</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>7</v>
@@ -2075,10 +2179,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>7</v>
@@ -2092,7 +2196,12 @@
       <c r="F19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="I19" s="6" t="s">
         <v>7</v>
       </c>
@@ -2102,337 +2211,380 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="C24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="6">
-        <v>1</v>
-      </c>
-      <c r="D33" s="6">
-        <v>1</v>
-      </c>
-      <c r="E33" s="6">
-        <v>1</v>
-      </c>
-      <c r="F33" s="6">
-        <v>1</v>
-      </c>
-      <c r="G33" s="6">
-        <v>20</v>
-      </c>
-      <c r="H33" s="6">
-        <v>20</v>
-      </c>
-      <c r="I33" s="6">
-        <v>20</v>
-      </c>
-      <c r="J33" s="6">
-        <v>20</v>
-      </c>
+      <c r="C33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>7</v>
@@ -2446,7 +2598,12 @@
       <c r="F34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="6"/>
+      <c r="G34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="I34" s="6" t="s">
         <v>7</v>
       </c>
@@ -2456,7 +2613,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>28</v>
@@ -2467,136 +2624,223 @@
       <c r="D35" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" s="6">
-        <v>28</v>
-      </c>
-      <c r="F36" s="6">
-        <v>28</v>
-      </c>
-      <c r="I36">
-        <v>2800</v>
-      </c>
-      <c r="J36">
-        <v>1400</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>7</v>
+        <v>27</v>
+      </c>
+      <c r="C37" s="6">
+        <v>1</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6">
+        <v>1</v>
+      </c>
+      <c r="F37" s="6">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6">
+        <v>20</v>
+      </c>
+      <c r="H37" s="6">
+        <v>20</v>
+      </c>
+      <c r="I37" s="6">
+        <v>20</v>
+      </c>
+      <c r="J37" s="6">
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="6">
-        <v>1</v>
-      </c>
-      <c r="G40" s="6">
-        <v>56</v>
-      </c>
-      <c r="H40">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="6">
+        <v>28</v>
+      </c>
+      <c r="F40" s="6">
+        <v>28</v>
+      </c>
+      <c r="I40">
+        <v>2800</v>
+      </c>
+      <c r="J40">
+        <v>1400</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" s="6" t="b">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C42" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="6">
+        <v>1</v>
+      </c>
+      <c r="G44" s="6">
+        <v>56</v>
+      </c>
+      <c r="H44">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E46" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F46" s="6" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>